<commit_message>
Combine ROIs for a subject
</commit_message>
<xml_diff>
--- a/rois/CombinedFreesurferLabels_reorg.xlsx
+++ b/rois/CombinedFreesurferLabels_reorg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogersbp/repo/fsthalconn/rois/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804F9F2C-2B20-8546-9C55-DE2D37B5E484}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB83D512-88B9-1141-8702-0A6A0D56BB03}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5700" yWindow="960" windowWidth="22720" windowHeight="16540" xr2:uid="{4D55D30D-0C4B-BD4E-977D-0921BE6881A2}"/>
   </bookViews>
@@ -577,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{103607CA-33ED-EF42-A8E5-68EA83D67222}">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -658,62 +658,82 @@
         <v>7007</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>13</v>
+      </c>
+    </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>11</v>
+        <v>1028</v>
       </c>
       <c r="E5">
-        <v>12</v>
+        <v>1002</v>
       </c>
       <c r="F5">
-        <v>13</v>
+        <v>1026</v>
+      </c>
+      <c r="G5">
+        <v>1014</v>
+      </c>
+      <c r="H5">
+        <v>1012</v>
+      </c>
+      <c r="I5">
+        <v>1027</v>
+      </c>
+      <c r="J5">
+        <v>1018</v>
+      </c>
+      <c r="K5">
+        <v>1019</v>
+      </c>
+      <c r="L5">
+        <v>1020</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>1028</v>
       </c>
       <c r="E6">
-        <v>1002</v>
+        <v>1014</v>
       </c>
       <c r="F6">
-        <v>1026</v>
-      </c>
-      <c r="G6">
-        <v>1014</v>
-      </c>
-      <c r="H6">
         <v>1012</v>
-      </c>
-      <c r="I6">
-        <v>1027</v>
-      </c>
-      <c r="J6">
-        <v>1018</v>
-      </c>
-      <c r="K6">
-        <v>1019</v>
-      </c>
-      <c r="L6">
-        <v>1020</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -724,16 +744,19 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="E7">
-        <v>1014</v>
+        <v>1018</v>
       </c>
       <c r="F7">
-        <v>1012</v>
+        <v>1019</v>
+      </c>
+      <c r="G7">
+        <v>1020</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -744,47 +767,53 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>1027</v>
+        <v>1002</v>
       </c>
       <c r="E8">
-        <v>1018</v>
-      </c>
-      <c r="F8">
-        <v>1019</v>
-      </c>
-      <c r="G8">
-        <v>1020</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D9">
-        <v>1002</v>
+        <v>1008</v>
       </c>
       <c r="E9">
-        <v>1026</v>
+        <v>1029</v>
+      </c>
+      <c r="F9">
+        <v>1025</v>
+      </c>
+      <c r="G9">
+        <v>1010</v>
+      </c>
+      <c r="H9">
+        <v>1023</v>
+      </c>
+      <c r="I9">
+        <v>1030</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>1008</v>
@@ -795,15 +824,6 @@
       <c r="F10">
         <v>1025</v>
       </c>
-      <c r="G10">
-        <v>1010</v>
-      </c>
-      <c r="H10">
-        <v>1023</v>
-      </c>
-      <c r="I10">
-        <v>1030</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -813,44 +833,56 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E11">
-        <v>1029</v>
-      </c>
-      <c r="F11">
-        <v>1025</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>1010</v>
+        <v>1030</v>
       </c>
       <c r="E12">
-        <v>1031</v>
+        <v>1034</v>
+      </c>
+      <c r="F12">
+        <v>1015</v>
+      </c>
+      <c r="G12">
+        <v>1007</v>
+      </c>
+      <c r="H12">
+        <v>1009</v>
+      </c>
+      <c r="I12">
+        <v>1016</v>
+      </c>
+      <c r="J12">
+        <v>1006</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <v>1030</v>
@@ -858,21 +890,6 @@
       <c r="E13">
         <v>1034</v>
       </c>
-      <c r="F13">
-        <v>1015</v>
-      </c>
-      <c r="G13">
-        <v>1007</v>
-      </c>
-      <c r="H13">
-        <v>1009</v>
-      </c>
-      <c r="I13">
-        <v>1016</v>
-      </c>
-      <c r="J13">
-        <v>1006</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -882,39 +899,42 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>1030</v>
+        <v>1015</v>
       </c>
       <c r="E14">
-        <v>1034</v>
+        <v>1007</v>
+      </c>
+      <c r="F14">
+        <v>1009</v>
+      </c>
+      <c r="G14">
+        <v>1016</v>
+      </c>
+      <c r="H14">
+        <v>1006</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D15">
-        <v>1015</v>
+        <v>1003</v>
       </c>
       <c r="E15">
-        <v>1007</v>
+        <v>1017</v>
       </c>
       <c r="F15">
-        <v>1009</v>
-      </c>
-      <c r="G15">
-        <v>1016</v>
-      </c>
-      <c r="H15">
-        <v>1006</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -925,19 +945,13 @@
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16">
-        <v>1003</v>
-      </c>
-      <c r="E16">
-        <v>1017</v>
-      </c>
-      <c r="F16">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -945,36 +959,65 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1021</v>
+      </c>
+      <c r="E17">
+        <v>1011</v>
+      </c>
+      <c r="F17">
+        <v>1013</v>
+      </c>
+      <c r="G17">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D18">
-        <v>1021</v>
+        <v>8103</v>
       </c>
       <c r="E18">
-        <v>1011</v>
-      </c>
-      <c r="F18">
-        <v>1013</v>
-      </c>
-      <c r="G18">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>8126</v>
+      </c>
+      <c r="E19">
+        <v>8127</v>
+      </c>
+      <c r="F19">
+        <v>8128</v>
+      </c>
+      <c r="G19">
+        <v>8129</v>
+      </c>
+      <c r="H19">
+        <v>8130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -982,16 +1025,13 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D20">
-        <v>8103</v>
-      </c>
-      <c r="E20">
-        <v>8108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -999,25 +1039,25 @@
         <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D21">
-        <v>8126</v>
+        <v>8105</v>
       </c>
       <c r="E21">
-        <v>8127</v>
+        <v>8106</v>
       </c>
       <c r="F21">
-        <v>8128</v>
+        <v>8104</v>
       </c>
       <c r="G21">
-        <v>8129</v>
+        <v>8117</v>
       </c>
       <c r="H21">
-        <v>8130</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1025,84 +1065,81 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D22">
-        <v>8133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8112</v>
+      </c>
+      <c r="E22">
+        <v>8113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D23">
-        <v>8105</v>
-      </c>
-      <c r="E23">
-        <v>8106</v>
-      </c>
-      <c r="F23">
-        <v>8104</v>
-      </c>
-      <c r="G23">
-        <v>8117</v>
-      </c>
-      <c r="H23">
-        <v>8118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D24">
-        <v>8112</v>
-      </c>
-      <c r="E24">
         <v>8113</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D25">
-        <v>8112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8120</v>
+      </c>
+      <c r="E25">
+        <v>8121</v>
+      </c>
+      <c r="F25">
+        <v>8122</v>
+      </c>
+      <c r="G25">
+        <v>8123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D26">
-        <v>8113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1110,22 +1147,13 @@
         <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D27">
-        <v>8120</v>
-      </c>
-      <c r="E27">
-        <v>8121</v>
-      </c>
-      <c r="F27">
-        <v>8122</v>
-      </c>
-      <c r="G27">
-        <v>8123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1133,455 +1161,512 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D28">
-        <v>8110</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D29">
-        <v>8115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+      <c r="E29">
+        <v>231</v>
+      </c>
+      <c r="F29">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D30">
-        <v>8109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7010</v>
+      </c>
+      <c r="E30">
+        <v>7001</v>
+      </c>
+      <c r="F30">
+        <v>7003</v>
+      </c>
+      <c r="G30">
+        <v>7015</v>
+      </c>
+      <c r="H30">
+        <v>7008</v>
+      </c>
+      <c r="I30">
+        <v>7006</v>
+      </c>
+      <c r="J30">
+        <v>7005</v>
+      </c>
+      <c r="K30">
+        <v>7007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>50</v>
+      </c>
+      <c r="E31">
+        <v>51</v>
+      </c>
+      <c r="F31">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D32">
-        <v>232</v>
+        <v>2028</v>
       </c>
       <c r="E32">
-        <v>231</v>
+        <v>2002</v>
       </c>
       <c r="F32">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2026</v>
+      </c>
+      <c r="G32">
+        <v>2014</v>
+      </c>
+      <c r="H32">
+        <v>2012</v>
+      </c>
+      <c r="I32">
+        <v>2027</v>
+      </c>
+      <c r="J32">
+        <v>2018</v>
+      </c>
+      <c r="K32">
+        <v>2019</v>
+      </c>
+      <c r="L32">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D33">
-        <v>7010</v>
+        <v>2028</v>
       </c>
       <c r="E33">
-        <v>7001</v>
+        <v>2014</v>
       </c>
       <c r="F33">
-        <v>7003</v>
-      </c>
-      <c r="G33">
-        <v>7015</v>
-      </c>
-      <c r="H33">
-        <v>7008</v>
-      </c>
-      <c r="I33">
-        <v>7006</v>
-      </c>
-      <c r="J33">
-        <v>7005</v>
-      </c>
-      <c r="K33">
-        <v>7007</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34">
+        <v>2027</v>
+      </c>
+      <c r="E34">
+        <v>2018</v>
+      </c>
+      <c r="F34">
+        <v>2019</v>
+      </c>
+      <c r="G34">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D35">
+        <v>2002</v>
+      </c>
+      <c r="E35">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>2008</v>
+      </c>
+      <c r="E36">
+        <v>2029</v>
+      </c>
+      <c r="F36">
+        <v>2025</v>
+      </c>
+      <c r="G36">
+        <v>2010</v>
+      </c>
+      <c r="H36">
+        <v>2023</v>
+      </c>
+      <c r="I36">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37">
+        <v>2008</v>
+      </c>
+      <c r="E37">
+        <v>2029</v>
+      </c>
+      <c r="F37">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38">
+        <v>2010</v>
+      </c>
+      <c r="E38">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39">
+        <v>2030</v>
+      </c>
+      <c r="E39">
+        <v>2034</v>
+      </c>
+      <c r="F39">
+        <v>2015</v>
+      </c>
+      <c r="G39">
+        <v>2007</v>
+      </c>
+      <c r="H39">
+        <v>2009</v>
+      </c>
+      <c r="I39">
+        <v>2016</v>
+      </c>
+      <c r="J39">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40">
+        <v>2030</v>
+      </c>
+      <c r="E40">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41">
+        <v>2015</v>
+      </c>
+      <c r="E41">
+        <v>2007</v>
+      </c>
+      <c r="F41">
+        <v>2009</v>
+      </c>
+      <c r="G41">
+        <v>2016</v>
+      </c>
+      <c r="H41">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>2003</v>
+      </c>
+      <c r="E42">
+        <v>2017</v>
+      </c>
+      <c r="F42">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44">
+        <v>2021</v>
+      </c>
+      <c r="E44">
+        <v>2011</v>
+      </c>
+      <c r="F44">
+        <v>2013</v>
+      </c>
+      <c r="G44">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s">
         <v>50</v>
       </c>
-      <c r="E35">
+      <c r="D45">
+        <v>8203</v>
+      </c>
+      <c r="E45">
+        <v>8208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C46" t="s">
         <v>51</v>
       </c>
-      <c r="F35">
+      <c r="D46">
+        <v>8226</v>
+      </c>
+      <c r="E46">
+        <v>8227</v>
+      </c>
+      <c r="F46">
+        <v>8228</v>
+      </c>
+      <c r="G46">
+        <v>8229</v>
+      </c>
+      <c r="H46">
+        <v>8230</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36">
-        <v>2028</v>
-      </c>
-      <c r="E36">
-        <v>2002</v>
-      </c>
-      <c r="F36">
-        <v>2026</v>
-      </c>
-      <c r="G36">
-        <v>2014</v>
-      </c>
-      <c r="H36">
-        <v>2012</v>
-      </c>
-      <c r="I36">
-        <v>2027</v>
-      </c>
-      <c r="J36">
-        <v>2018</v>
-      </c>
-      <c r="K36">
-        <v>2019</v>
-      </c>
-      <c r="L36">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>2</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37">
-        <v>2028</v>
-      </c>
-      <c r="E37">
-        <v>2014</v>
-      </c>
-      <c r="F37">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>2</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38">
-        <v>2027</v>
-      </c>
-      <c r="E38">
-        <v>2018</v>
-      </c>
-      <c r="F38">
-        <v>2019</v>
-      </c>
-      <c r="G38">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>2</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39">
-        <v>2002</v>
-      </c>
-      <c r="E39">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40">
-        <v>2008</v>
-      </c>
-      <c r="E40">
-        <v>2029</v>
-      </c>
-      <c r="F40">
-        <v>2025</v>
-      </c>
-      <c r="G40">
-        <v>2010</v>
-      </c>
-      <c r="H40">
-        <v>2023</v>
-      </c>
-      <c r="I40">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41">
-        <v>2008</v>
-      </c>
-      <c r="E41">
-        <v>2029</v>
-      </c>
-      <c r="F41">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>2</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42">
-        <v>2010</v>
-      </c>
-      <c r="E42">
-        <v>2031</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" t="s">
-        <v>21</v>
-      </c>
-      <c r="D43">
-        <v>2030</v>
-      </c>
-      <c r="E43">
-        <v>2034</v>
-      </c>
-      <c r="F43">
-        <v>2015</v>
-      </c>
-      <c r="G43">
-        <v>2007</v>
-      </c>
-      <c r="H43">
-        <v>2009</v>
-      </c>
-      <c r="I43">
-        <v>2016</v>
-      </c>
-      <c r="J43">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>2</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" t="s">
-        <v>48</v>
-      </c>
-      <c r="D44">
-        <v>2030</v>
-      </c>
-      <c r="E44">
-        <v>2034</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45">
-        <v>2015</v>
-      </c>
-      <c r="E45">
-        <v>2007</v>
-      </c>
-      <c r="F45">
-        <v>2009</v>
-      </c>
-      <c r="G45">
-        <v>2016</v>
-      </c>
-      <c r="H45">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46">
-        <v>2003</v>
-      </c>
-      <c r="E46">
-        <v>2017</v>
-      </c>
-      <c r="F46">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
       <c r="D47">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+        <v>8233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D48">
-        <v>2021</v>
+        <v>8205</v>
       </c>
       <c r="E48">
-        <v>2011</v>
+        <v>8206</v>
       </c>
       <c r="F48">
-        <v>2013</v>
+        <v>8204</v>
       </c>
       <c r="G48">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8217</v>
+      </c>
+      <c r="H48">
+        <v>8218</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49">
+        <v>8212</v>
+      </c>
+      <c r="E49">
+        <v>8213</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D50">
-        <v>8203</v>
-      </c>
-      <c r="E50">
-        <v>8208</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D51">
-        <v>8226</v>
-      </c>
-      <c r="E51">
-        <v>8227</v>
-      </c>
-      <c r="F51">
-        <v>8228</v>
-      </c>
-      <c r="G51">
-        <v>8229</v>
-      </c>
-      <c r="H51">
-        <v>8230</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8213</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -1589,13 +1674,22 @@
         <v>14</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="D52">
-        <v>8233</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8220</v>
+      </c>
+      <c r="E52">
+        <v>8221</v>
+      </c>
+      <c r="F52">
+        <v>8222</v>
+      </c>
+      <c r="G52">
+        <v>8223</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -1603,25 +1697,13 @@
         <v>14</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D53">
-        <v>8205</v>
-      </c>
-      <c r="E53">
-        <v>8206</v>
-      </c>
-      <c r="F53">
-        <v>8204</v>
-      </c>
-      <c r="G53">
-        <v>8217</v>
-      </c>
-      <c r="H53">
-        <v>8218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -1629,105 +1711,23 @@
         <v>14</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D54">
-        <v>8212</v>
-      </c>
-      <c r="E54">
-        <v>8213</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>8215</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D55">
-        <v>8212</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>2</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56">
-        <v>8213</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>1</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57">
-        <v>8220</v>
-      </c>
-      <c r="E57">
-        <v>8221</v>
-      </c>
-      <c r="F57">
-        <v>8222</v>
-      </c>
-      <c r="G57">
-        <v>8223</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58">
-        <v>8210</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59">
-        <v>8215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60">
         <v>8209</v>
       </c>
     </row>

</xml_diff>